<commit_message>
Ajustes perfil y ejemplos Encounter y Coverage y generacion perfil y ejemplo recurso ServiceRequest
Ajustes perfil y ejemplos Encounter y Coverage y generacion perfil y ejemplo recurso ServiceRequest - 17022021.
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-RateModality.xlsx
+++ b/fhir/indisa/StructureDefinition-RateModality.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="111">
   <si>
     <t>Path</t>
   </si>
@@ -304,6 +304,10 @@
   </si>
   <si>
     <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Note that FHIR strings SHALL NOT exceed 1MB in size
+Possible values:  abierta / libre elección, cerrada/preferente, GES-CAEC.</t>
   </si>
   <si>
     <t>Need to refer to a particular code in the system.</t>
@@ -1604,9 +1608,11 @@
       <c r="L11" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" t="s" s="2">
+        <v>93</v>
+      </c>
       <c r="N11" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>37</v>
@@ -1655,7 +1661,7 @@
         <v>37</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>38</v>
@@ -1670,12 +1676,12 @@
         <v>68</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1701,14 +1707,14 @@
         <v>45</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>37</v>
@@ -1757,7 +1763,7 @@
         <v>37</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>38</v>
@@ -1772,12 +1778,12 @@
         <v>68</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1800,19 +1806,19 @@
         <v>76</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>37</v>
@@ -1861,7 +1867,7 @@
         <v>37</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>38</v>
@@ -1876,7 +1882,7 @@
         <v>68</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>